<commit_message>
BUG: Fix read_excel w/parse_cols & empty dataset (#23661)
Closes gh-9208.
</commit_message>
<xml_diff>
--- a/pandas/tests/io/data/test1.xlsx
+++ b/pandas/tests/io/data/test1.xlsx
@@ -1,14 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21721"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21001"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Beano\Repositories\pandas\pandas\tests\io\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A80AB08-DD4C-4F74-A488-F01DCF0B07AA}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="-20" windowWidth="29560" windowHeight="24100" tabRatio="500"/>
+    <workbookView xWindow="84" yWindow="-24" windowWidth="29556" windowHeight="24096" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="130407" concurrentCalc="0"/>
   <extLst>
@@ -20,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="10">
   <si>
     <t>A</t>
   </si>
@@ -48,12 +55,18 @@
   <si>
     <t>ignore</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>F</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -93,6 +106,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -417,17 +438,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" workbookViewId="0"/>
+    <sheetView view="pageLayout" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" customWidth="1"/>
+    <col min="1" max="1" width="19.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -441,7 +462,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>35066</v>
       </c>
@@ -458,7 +479,7 @@
         <v>-1.1597380616899999</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>35067</v>
       </c>
@@ -475,7 +496,7 @@
         <v>0.212549316967</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>35068</v>
       </c>
@@ -492,7 +513,7 @@
         <v>1.3462704195199999</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>35069</v>
       </c>
@@ -509,7 +530,7 @@
         <v>0.67525259227000001</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>35070</v>
       </c>
@@ -526,7 +547,7 @@
         <v>0.103468562917</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>35073</v>
       </c>
@@ -543,7 +564,7 @@
         <v>1.0627820613000001</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>35074</v>
       </c>
@@ -563,7 +584,7 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="1" OnePage="0" WScale="0"/>
@@ -573,16 +594,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView view="pageLayout" workbookViewId="0">
       <selection sqref="A1:E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -596,7 +617,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>4</v>
       </c>
@@ -610,7 +631,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>35066</v>
       </c>
@@ -627,7 +648,7 @@
         <v>-1.1597380616899999</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>35067</v>
       </c>
@@ -644,7 +665,7 @@
         <v>0.212549316967</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>35068</v>
       </c>
@@ -661,7 +682,7 @@
         <v>1.3462704195199999</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>35069</v>
       </c>
@@ -678,7 +699,7 @@
         <v>0.67525259227000001</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>35070</v>
       </c>
@@ -695,7 +716,7 @@
         <v>0.103468562917</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>35073</v>
       </c>
@@ -712,7 +733,7 @@
         <v>1.0627820613000001</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>35074</v>
       </c>
@@ -732,11 +753,46 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="1" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4669757C-F7B6-4CFC-9F46-A8DF37DF746B}">
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
TST: Test unnamed columns with index_col for Excel (#23874)
</commit_message>
<xml_diff>
--- a/pandas/tests/io/data/test1.xlsx
+++ b/pandas/tests/io/data/test1.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Beano\Repositories\pandas\pandas\tests\io\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A80AB08-DD4C-4F74-A488-F01DCF0B07AA}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B9007CB-C74A-4E7F-8E16-6EDF2B37F435}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="84" yWindow="-24" windowWidth="29556" windowHeight="24096" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="84" yWindow="-24" windowWidth="29556" windowHeight="24096" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="130407" concurrentCalc="0"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="18">
   <si>
     <t>A</t>
   </si>
@@ -61,13 +62,37 @@
   </si>
   <si>
     <t>F</t>
+  </si>
+  <si>
+    <t>col1</t>
+  </si>
+  <si>
+    <t>col2</t>
+  </si>
+  <si>
+    <t>i1</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>i2</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>y</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
@@ -75,6 +100,14 @@
     <font>
       <sz val="8"/>
       <name val="Verdana"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -85,7 +118,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -93,13 +126,31 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -766,7 +817,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4669757C-F7B6-4CFC-9F46-A8DF37DF746B}">
   <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
@@ -795,4 +846,49 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{624CF529-5128-482A-A33B-732E2FE6972F}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" ht="14.4" x14ac:dyDescent="0.2">
+      <c r="B1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="14.4" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="14.4" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Openpyxl engine for reading excel files (#25092)
</commit_message>
<xml_diff>
--- a/pandas/tests/io/data/test1.xlsx
+++ b/pandas/tests/io/data/test1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21001"/>
-  <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Beano\Repositories\pandas\pandas\tests\io\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/williamayd/clones/pandas/pandas/tests/io/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B9007CB-C74A-4E7F-8E16-6EDF2B37F435}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{531BDF74-4C20-AC4F-B21A-F90470D62DAB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="84" yWindow="-24" windowWidth="29556" windowHeight="24096" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1760" yWindow="760" windowWidth="27640" windowHeight="16060" xr2:uid="{83D80846-740D-F245-84E4-070D53ACA2AD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,10 +18,16 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="130407" concurrentCalc="0"/>
+  <calcPr calcId="181029" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -43,19 +49,19 @@
   </si>
   <si>
     <t>col</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
     <t>we</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
     <t>should</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
     <t>ignore</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
     <t>E</t>
@@ -92,14 +98,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <sz val="10"/>
-      <name val="Verdana"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <name val="Verdana"/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -148,7 +153,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -156,7 +161,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -179,44 +184,44 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="1F497D"/>
+        <a:srgbClr val="44546A"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="EEECE1"/>
+        <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4F81BD"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="C0504D"/>
+        <a:srgbClr val="ED7D31"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="9BBB59"/>
+        <a:srgbClr val="A5A5A5"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="8064A2"/>
+        <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4BACC6"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="F79646"/>
+        <a:srgbClr val="70AD47"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0000FF"/>
+        <a:srgbClr val="0563C1"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="800080"/>
+        <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="等线 Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -244,14 +249,31 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="等线"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -279,6 +301,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -290,213 +329,156 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-                <a:satMod val="300000"/>
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="35000">
+            <a:gs pos="50000">
               <a:schemeClr val="phClr">
-                <a:tint val="37000"/>
-                <a:satMod val="300000"/>
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
-                <a:satMod val="350000"/>
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="100000"/>
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
                 <a:shade val="100000"/>
-                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-                <a:shade val="100000"/>
-                <a:satMod val="350000"/>
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="0"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr">
-              <a:shade val="95000"/>
-              <a:satMod val="105000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
+                <a:alpha val="63000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-          <a:scene3d>
-            <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
-            </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
-            </a:lightRig>
-          </a:scene3d>
-          <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
-          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="40000"/>
-                <a:satMod val="350000"/>
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="40000">
+            <a:gs pos="50000">
               <a:schemeClr val="phClr">
-                <a:tint val="45000"/>
-                <a:shade val="99000"/>
-                <a:satMod val="350000"/>
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="20000"/>
-                <a:satMod val="255000"/>
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
-          </a:path>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="80000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="30000"/>
-                <a:satMod val="200000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-          </a:path>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults>
-    <a:spDef>
-      <a:spPr/>
-      <a:bodyPr/>
-      <a:lstStyle/>
-      <a:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="3">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </a:style>
-    </a:spDef>
-    <a:lnDef>
-      <a:spPr/>
-      <a:bodyPr/>
-      <a:lstStyle/>
-      <a:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </a:style>
-    </a:lnDef>
-  </a:objectDefaults>
+  <a:objectDefaults/>
   <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCFCA61B-52C3-834A-BF4F-09112C347348}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView view="pageLayout" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.26953125" customWidth="1"/>
+    <col min="1" max="1" width="11.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
@@ -515,7 +497,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
-        <v>35066</v>
+        <v>36528</v>
       </c>
       <c r="B2">
         <v>0.98026851377699997</v>
@@ -532,7 +514,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
-        <v>35067</v>
+        <v>36529</v>
       </c>
       <c r="B3">
         <v>1.04791624281</v>
@@ -549,7 +531,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
-        <v>35068</v>
+        <v>36530</v>
       </c>
       <c r="B4">
         <v>0.49858088570499998</v>
@@ -566,7 +548,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
-        <v>35069</v>
+        <v>36531</v>
       </c>
       <c r="B5">
         <v>1.1202015186900001</v>
@@ -583,7 +565,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
-        <v>35070</v>
+        <v>36532</v>
       </c>
       <c r="B6">
         <v>-0.48709439946299998</v>
@@ -600,7 +582,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
-        <v>35073</v>
+        <v>36535</v>
       </c>
       <c r="B7">
         <v>0.83664867166599999</v>
@@ -617,7 +599,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
-        <v>35074</v>
+        <v>36536</v>
       </c>
       <c r="B8">
         <v>-0.157160753327</v>
@@ -633,26 +615,19 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="1" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B48E2057-3592-C44A-86EF-7E23838A9FFC}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView view="pageLayout" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
@@ -684,7 +659,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
-        <v>35066</v>
+        <v>36528</v>
       </c>
       <c r="B3">
         <v>0.98026851377699997</v>
@@ -701,7 +676,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
-        <v>35067</v>
+        <v>36529</v>
       </c>
       <c r="B4">
         <v>1.04791624281</v>
@@ -718,7 +693,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
-        <v>35068</v>
+        <v>36530</v>
       </c>
       <c r="B5">
         <v>0.49858088570499998</v>
@@ -735,7 +710,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
-        <v>35069</v>
+        <v>36531</v>
       </c>
       <c r="B6">
         <v>1.1202015186900001</v>
@@ -752,7 +727,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
-        <v>35070</v>
+        <v>36532</v>
       </c>
       <c r="B7">
         <v>-0.48709439946299998</v>
@@ -769,7 +744,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
-        <v>35073</v>
+        <v>36535</v>
       </c>
       <c r="B8">
         <v>0.83664867166599999</v>
@@ -786,7 +761,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
-        <v>35074</v>
+        <v>36536</v>
       </c>
       <c r="B9">
         <v>-0.157160753327</v>
@@ -802,26 +777,19 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="1" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4669757C-F7B6-4CFC-9F46-A8DF37DF746B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B151EF2-7DAF-3542-B021-F4540923EAFF}">
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -849,16 +817,16 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{624CF529-5128-482A-A33B-732E2FE6972F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B305A25-F2CC-5E4E-B3AD-49DEDB1C3E16}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" ht="14.4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B1" s="2" t="s">
         <v>10</v>
       </c>
@@ -866,7 +834,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="14.4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>12</v>
       </c>
@@ -877,7 +845,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="14.4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>15</v>
       </c>

</xml_diff>